<commit_message>
clean up before submission validation paper
</commit_message>
<xml_diff>
--- a/script/bandtransform.xlsx
+++ b/script/bandtransform.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\Remote-Sensing-of-Albedo\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF00DF3D-111D-4437-8007-9453E670AC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54429C5B-2809-4CE6-B890-C97C44217497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="2490" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43980" yWindow="4095" windowWidth="28800" windowHeight="15375" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransformAll" sheetId="3" r:id="rId1"/>
     <sheet name="albedo paper1" sheetId="1" r:id="rId2"/>
     <sheet name="albedo paper2" sheetId="2" r:id="rId3"/>
+    <sheet name="satmission" sheetId="4" r:id="rId4"/>
+    <sheet name="all" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="115">
   <si>
     <t>Band</t>
   </si>
@@ -192,16 +194,232 @@
   </si>
   <si>
     <t>L8=0.7479*L9+0.0162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean
+Difference </t>
+  </si>
+  <si>
+    <t>Mean Difference 
+L8-L9</t>
+  </si>
+  <si>
+    <t>satellite</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>Landsat 4</t>
+  </si>
+  <si>
+    <t>Landsat 5</t>
+  </si>
+  <si>
+    <t>Landsat 7</t>
+  </si>
+  <si>
+    <t>Landsat 8</t>
+  </si>
+  <si>
+    <t>Sentinel 2</t>
+  </si>
+  <si>
+    <t>Landsat 9</t>
+  </si>
+  <si>
+    <t>band</t>
+  </si>
+  <si>
+    <t>band name</t>
+  </si>
+  <si>
+    <t>sr band name</t>
+  </si>
+  <si>
+    <t>wavelength (nm) 1</t>
+  </si>
+  <si>
+    <t>wavelength (nm) 2</t>
+  </si>
+  <si>
+    <t>resolution (m)</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Coastal aerosol</t>
+  </si>
+  <si>
+    <t>SR_B1</t>
+  </si>
+  <si>
+    <t>SR_B2</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>SR_B3</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>SR_B4</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>SR_B5</t>
+  </si>
+  <si>
+    <t>darkcyan</t>
+  </si>
+  <si>
+    <t>SWIR 1</t>
+  </si>
+  <si>
+    <t>SR_B6</t>
+  </si>
+  <si>
+    <t>darkmagenta</t>
+  </si>
+  <si>
+    <t>SWIR 2</t>
+  </si>
+  <si>
+    <t>SR_B7</t>
+  </si>
+  <si>
+    <t>olivedrab</t>
+  </si>
+  <si>
+    <t>Panchromatic</t>
+  </si>
+  <si>
+    <t>Cirrus</t>
+  </si>
+  <si>
+    <t>TIRS 1</t>
+  </si>
+  <si>
+    <t>TIRS 2</t>
+  </si>
+  <si>
+    <t>brightness temperature</t>
+  </si>
+  <si>
+    <t>Landsat 4/5</t>
+  </si>
+  <si>
+    <t>Aerosols</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>Red Edge 1</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>Red Edge 2</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>Red Edge 3</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>Red Edge 4</t>
+  </si>
+  <si>
+    <t>B8A</t>
+  </si>
+  <si>
+    <t>Water vapor</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>Landsat 8/9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,13 +445,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,7 +788,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -562,90 +797,90 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="10">
         <v>87023</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="10">
         <v>0.8</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="10">
         <v>0.1358</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="10">
         <v>7093591</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="10">
         <v>0.8</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <v>0.14069999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <v>2273220</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="10">
         <v>0.85</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="10">
         <v>0.10680000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -654,90 +889,90 @@
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="10">
         <v>151161</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="10">
         <v>0.77</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="10">
         <v>0.12859999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <v>10496934</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="10">
         <v>0.78</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="10">
         <v>0.1249</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="10">
         <v>3399280</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="10">
         <v>0.83</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="10">
         <v>0.1032</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -746,90 +981,90 @@
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="10">
         <v>174402</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="10">
         <v>0.74</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="10">
         <v>0.13250000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="10">
         <v>13207115</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="10">
         <v>0.77</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="10">
         <v>0.1308</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="10">
         <v>4470845</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="10">
         <v>0.82</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="10">
         <v>0.1031</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -838,90 +1073,90 @@
       <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="10">
         <v>277074</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="10">
         <v>0.78</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="10">
         <v>0.14319999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="10">
         <v>32157181</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="10">
         <v>0.85</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="10">
         <v>0.1048</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="10">
         <v>14061397</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="10">
         <v>0.88</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="10">
         <v>8.77E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -930,90 +1165,90 @@
       <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="10">
         <v>261157</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="10">
         <v>0.59</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="10">
         <v>3.61E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="10">
         <v>27130955</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="10">
         <v>0.76</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="10">
         <v>2.3E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="10">
         <v>12264530</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="10">
         <v>0.69</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="10">
         <v>2.5700000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1022,140 +1257,90 @@
       <c r="C32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="10">
         <v>367345</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="10">
         <v>0.78</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="10">
         <v>3.09E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="10">
         <v>35816180</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="10">
         <v>0.83</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="10">
         <v>2.06E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="10">
         <v>17411684</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="10">
         <v>0.79</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="10">
         <v>2.4799999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
@@ -1166,6 +1351,56 @@
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1173,22 +1408,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="A1:F25"/>
+      <selection activeCell="C5" sqref="A1:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1207,9 +1443,12 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1218,60 +1457,68 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="10">
         <v>87023</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="10">
         <v>0.8</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="10">
         <v>0.1358</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="G2" s="10">
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="10">
         <v>7093591</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="10">
         <v>0.8</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <v>0.14069999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="G4" s="10">
+        <v>8.4199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1280,60 +1527,68 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <v>151161</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="10">
         <v>0.77</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="10">
         <v>0.12859999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="G6" s="10">
+        <v>5.6500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="10">
         <v>10496934</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="10">
         <v>0.78</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="10">
         <v>0.1249</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="G8" s="10">
+        <v>6.2300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1342,60 +1597,68 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <v>174402</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="10">
         <v>0.74</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="10">
         <v>0.13250000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="G10" s="10">
+        <v>4.7399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="10">
         <v>13207115</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="10">
         <v>0.77</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="10">
         <v>0.1308</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="G12" s="10">
+        <v>7.2599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1404,60 +1667,68 @@
       <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="10">
         <v>277074</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="10">
         <v>0.78</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="10">
         <v>0.14319999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="G14" s="10">
+        <v>5.9499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="10">
         <v>32157181</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="10">
         <v>0.85</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="10">
         <v>0.1048</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="G16" s="10">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1466,60 +1737,68 @@
       <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="10">
         <v>261157</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="10">
         <v>0.59</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="10">
         <v>3.61E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="G18" s="10">
+        <v>-1.35E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="10">
         <v>27130955</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="10">
         <v>0.76</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="10">
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="G20" s="10">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1528,60 +1807,115 @@
       <c r="C22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="10">
         <v>367345</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="10">
         <v>0.78</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="10">
         <v>3.09E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="G22" s="10">
+        <v>1.15E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="10">
         <v>35816180</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="10">
         <v>0.83</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="10">
         <v>2.06E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="G24" s="10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="54">
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
@@ -1589,52 +1923,18 @@
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11018545-AB6F-43B8-BEE6-8CF2EB1D3C6B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,9 +1944,10 @@
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1665,9 +1966,12 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1676,30 +1980,34 @@
       <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="10">
         <v>2273220</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="10">
         <v>0.85</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="10">
         <v>0.10680000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="G2" s="10">
+        <v>6.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1708,30 +2016,34 @@
       <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="10">
         <v>3399280</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="10">
         <v>0.83</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <v>0.1032</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="G4" s="10">
+        <v>4.3E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1740,30 +2052,34 @@
       <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <v>4470845</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="10">
         <v>0.82</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="10">
         <v>0.1031</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="G6" s="10">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1772,30 +2088,34 @@
       <c r="C8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="10">
         <v>14061397</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="10">
         <v>0.88</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="10">
         <v>8.77E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="G8" s="10">
+        <v>9.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1804,30 +2124,34 @@
       <c r="C10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <v>12264530</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="10">
         <v>0.69</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="10">
         <v>2.5700000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="G10" s="10">
+        <v>3.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1836,30 +2160,93 @@
       <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="10">
         <v>17411684</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="10">
         <v>0.79</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="10">
         <v>2.4799999999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="G12" s="10">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="31">
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
@@ -1868,24 +2255,1194 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F722F589-A409-47EA-A297-82807F3FCD74}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5">
+        <v>30185</v>
+      </c>
+      <c r="C2" s="4">
+        <v>34317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="5">
+        <v>30757</v>
+      </c>
+      <c r="C3" s="5">
+        <v>41034</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5">
+        <v>36161</v>
+      </c>
+      <c r="C4" s="5">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5">
+        <v>41375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="5">
+        <v>42822</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F94B49F-57E8-483E-8B6F-503436125B2F}">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="7">
+        <v>430</v>
+      </c>
+      <c r="F2" s="6">
+        <v>450</v>
+      </c>
+      <c r="G2" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="6">
+        <v>450</v>
+      </c>
+      <c r="F3" s="6">
+        <v>510</v>
+      </c>
+      <c r="G3" s="6">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="6">
+        <v>530</v>
+      </c>
+      <c r="F4" s="6">
+        <v>590</v>
+      </c>
+      <c r="G4" s="6">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="6">
+        <v>640</v>
+      </c>
+      <c r="F5" s="6">
+        <v>670</v>
+      </c>
+      <c r="G5" s="6">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="6">
+        <v>850</v>
+      </c>
+      <c r="F6" s="6">
+        <v>880</v>
+      </c>
+      <c r="G6" s="6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1570</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1650</v>
+      </c>
+      <c r="G7" s="6">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2110</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2290</v>
+      </c>
+      <c r="G8" s="6">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="6">
+        <v>500</v>
+      </c>
+      <c r="F9" s="6">
+        <v>680</v>
+      </c>
+      <c r="G9" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6">
+        <v>1360</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1380</v>
+      </c>
+      <c r="G10" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6">
+        <v>10600</v>
+      </c>
+      <c r="F11" s="6">
+        <v>11190</v>
+      </c>
+      <c r="G11" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6">
+        <v>11500</v>
+      </c>
+      <c r="F12" s="6">
+        <v>12510</v>
+      </c>
+      <c r="G12" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="7">
+        <v>450</v>
+      </c>
+      <c r="F13" s="6">
+        <v>520</v>
+      </c>
+      <c r="G13" s="6">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="6">
+        <v>520</v>
+      </c>
+      <c r="F14" s="6">
+        <v>600</v>
+      </c>
+      <c r="G14" s="6">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="6">
+        <v>630</v>
+      </c>
+      <c r="F15" s="6">
+        <v>690</v>
+      </c>
+      <c r="G15" s="6">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="6">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="6">
+        <v>770</v>
+      </c>
+      <c r="F16" s="6">
+        <v>900</v>
+      </c>
+      <c r="G16" s="6">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="6">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1550</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1750</v>
+      </c>
+      <c r="G17" s="6">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="6">
+        <v>6</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="6">
+        <v>10400</v>
+      </c>
+      <c r="F18" s="6">
+        <v>12500</v>
+      </c>
+      <c r="G18" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="6">
+        <v>2090</v>
+      </c>
+      <c r="F19" s="6">
+        <v>2350</v>
+      </c>
+      <c r="G19" s="6">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="6">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="6">
+        <v>520</v>
+      </c>
+      <c r="F20" s="6">
+        <v>900</v>
+      </c>
+      <c r="G20" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="7">
+        <v>450</v>
+      </c>
+      <c r="F21" s="6">
+        <v>520</v>
+      </c>
+      <c r="G21" s="6">
+        <v>30</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="6">
+        <v>520</v>
+      </c>
+      <c r="F22" s="6">
+        <v>600</v>
+      </c>
+      <c r="G22" s="6">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="6">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="6">
+        <v>630</v>
+      </c>
+      <c r="F23" s="6">
+        <v>690</v>
+      </c>
+      <c r="G23" s="6">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="6">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="6">
+        <v>760</v>
+      </c>
+      <c r="F24" s="6">
+        <v>900</v>
+      </c>
+      <c r="G24" s="6">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="6">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1550</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1750</v>
+      </c>
+      <c r="G25" s="6">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="6">
+        <v>10400</v>
+      </c>
+      <c r="F26" s="6">
+        <v>12500</v>
+      </c>
+      <c r="G26" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="6">
+        <v>7</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="6">
+        <v>2080</v>
+      </c>
+      <c r="F27" s="6">
+        <v>2350</v>
+      </c>
+      <c r="G27" s="6">
+        <v>30</v>
+      </c>
+      <c r="H27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="6">
+        <v>433</v>
+      </c>
+      <c r="F28" s="6">
+        <v>453</v>
+      </c>
+      <c r="G28" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="6">
+        <v>457.5</v>
+      </c>
+      <c r="F29" s="6">
+        <v>522.5</v>
+      </c>
+      <c r="G29" s="6">
+        <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="6">
+        <v>3</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="6">
+        <v>542.5</v>
+      </c>
+      <c r="F30" s="6">
+        <v>577.5</v>
+      </c>
+      <c r="G30" s="6">
+        <v>10</v>
+      </c>
+      <c r="H30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="6">
+        <v>4</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="6">
+        <v>650</v>
+      </c>
+      <c r="F31" s="6">
+        <v>680</v>
+      </c>
+      <c r="G31" s="6">
+        <v>10</v>
+      </c>
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6">
+        <v>5</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="6">
+        <v>697.5</v>
+      </c>
+      <c r="F32" s="6">
+        <v>712.5</v>
+      </c>
+      <c r="G32" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="6">
+        <v>6</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="6">
+        <v>732.5</v>
+      </c>
+      <c r="F33" s="6">
+        <v>747.5</v>
+      </c>
+      <c r="G33" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="6">
+        <v>7</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="6">
+        <v>773</v>
+      </c>
+      <c r="F34" s="6">
+        <v>793</v>
+      </c>
+      <c r="G34" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="6">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="6">
+        <v>784.5</v>
+      </c>
+      <c r="F35" s="6">
+        <v>899.5</v>
+      </c>
+      <c r="G35" s="6">
+        <v>10</v>
+      </c>
+      <c r="H35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="6">
+        <v>855</v>
+      </c>
+      <c r="F36" s="6">
+        <v>875</v>
+      </c>
+      <c r="G36" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="6">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="6">
+        <v>935</v>
+      </c>
+      <c r="F37" s="6">
+        <v>955</v>
+      </c>
+      <c r="G37" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="6">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1360</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1390</v>
+      </c>
+      <c r="G38" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="6">
+        <v>11</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1565</v>
+      </c>
+      <c r="F39" s="6">
+        <v>1655</v>
+      </c>
+      <c r="G39" s="6">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="6">
+        <v>12</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="6">
+        <v>2100</v>
+      </c>
+      <c r="F40" s="6">
+        <v>2280</v>
+      </c>
+      <c r="G40" s="6">
+        <v>20</v>
+      </c>
+      <c r="H40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>